<commit_message>
Changed model from gemma3:27b to llava
</commit_message>
<xml_diff>
--- a/ScriptData/ScriptOutput.xlsx
+++ b/ScriptData/ScriptOutput.xlsx
@@ -1,44 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilia\Documents\HTW\Master WI\3 - Semester\Informatik und Gesellschaft\ProjectMasterFolder\ScriptData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28272DC6-6FD5-4D0B-AF63-BF4389708926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>TestA</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>TestB</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>TestC</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,17 +58,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -119,7 +114,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -153,6 +148,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -187,9 +183,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -362,38 +359,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>